<commit_message>
20211130 CRE21-020	To include the School Code in the Pre-Authorization Checking File (for both PPP-PS and PPP-KG)
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0001-PreAuthorization_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0001-PreAuthorization_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-016 (To update the format of the Pre Authorization Checking File)\Front-end\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-020 (Add School Code to Pre-Auth)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Residential Care Home Seasonal Influenza Vaccination for Health Care Worker</t>
   </si>
@@ -269,6 +269,14 @@
   </si>
   <si>
     <t>Selected</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To include the School Code in the Pre-Authorization Checking File (for both PPP-PS and PPP-KG)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1065,7 +1073,7 @@
         <v/>
       </c>
       <c r="K3" s="5" t="str">
-        <f>IF(LEN(K4) &gt; 0,"RCH Code","")</f>
+        <f>IF(LEN(K4) &gt; 0,IF(LEN(L4) &gt; 0,"RCH Code","School Code"),"")</f>
         <v/>
       </c>
       <c r="L3" s="5" t="str">
@@ -1231,7 +1239,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1347,6 +1355,20 @@
         <v>44162</v>
       </c>
     </row>
+    <row r="10" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>7</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="24">
+        <v>44530</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>